<commit_message>
adjusted max for dependency
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/GMI KPI Template v0.2.xlsx
+++ b/Projects/GMIUS/Data/GMI KPI Template v0.2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="155">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -509,7 +509,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -531,12 +531,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -640,12 +634,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -656,10 +650,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -674,7 +664,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,7 +672,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,19 +684,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,18 +781,20 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.3962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="108.674074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.3555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.6925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="111.518518518519"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,8 +1520,11 @@
       <c r="A38" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>58</v>
+      </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1604,17 +1599,17 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="D38 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,15 +1665,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D38 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,52 +1717,52 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="D38 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="9" t="n">
+      <c r="B1" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="n">
+      <c r="C1" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="n">
+      <c r="D1" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="n">
+      <c r="E1" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="n">
+      <c r="F1" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="n">
+      <c r="G1" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="n">
+      <c r="H1" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="n">
+      <c r="I1" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="n">
+      <c r="J1" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="n">
+      <c r="K1" s="8" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="9" t="n">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1788,7 +1783,7 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="9" t="n">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1811,7 +1806,7 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="9" t="n">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1836,7 +1831,7 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="9" t="n">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1863,7 +1858,7 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="9" t="n">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1892,7 +1887,7 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="9" t="n">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1923,7 +1918,7 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="9" t="n">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1956,7 +1951,7 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2009,13 +2004,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D38 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2037,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>120</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2050,7 +2045,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -2061,7 +2056,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>122</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -2069,7 +2064,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="82.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>123</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -2077,7 +2072,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2100,30 +2095,30 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="D38 D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.2518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.5259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,7 +2208,7 @@
       <c r="C2" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -2222,7 +2217,7 @@
       <c r="F2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>150</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -2234,7 +2229,7 @@
       <c r="J2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>151</v>
       </c>
       <c r="L2" s="0" t="s">
@@ -2249,7 +2244,7 @@
       <c r="O2" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="0" t="s">
@@ -2261,7 +2256,7 @@
       <c r="S2" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="V2" s="0" t="s">
@@ -2270,7 +2265,7 @@
       <c r="W2" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="X2" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2293,15 +2288,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="1" sqref="D38 I28"/>
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,13 +2314,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -2333,10 +2328,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>150</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -2347,10 +2342,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -2361,13 +2356,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>152</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -2375,24 +2370,24 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>152</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2415,14 +2410,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="D38 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.9555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.2296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,18 +2517,19 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="1" sqref="D38 C22"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.0518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2626,7 +2623,7 @@
       <c r="B7" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -2640,7 +2637,7 @@
       <c r="B8" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -2654,7 +2651,7 @@
       <c r="B9" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -2668,7 +2665,7 @@
       <c r="B10" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -2682,7 +2679,7 @@
       <c r="B11" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -2696,7 +2693,7 @@
       <c r="B12" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -2722,15 +2719,17 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D38 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,23 +2857,24 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D38 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2882,10 +2882,10 @@
       <c r="A2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="1"/>
@@ -2909,13 +2909,14 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="D38 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.3962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.3555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,26 +2928,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2969,12 +2970,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D38 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2986,8 +2988,8 @@
       <c r="A2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="0" t="s">
         <v>95</v>
       </c>
@@ -3011,15 +3013,16 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="D38 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.9185185185185"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.1888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,12 +3046,12 @@
       <c r="C2" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3071,12 +3074,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="D38 E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,10 +3098,10 @@
       <c r="A2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>